<commit_message>
Plotting state estimation and smoothing results
</commit_message>
<xml_diff>
--- a/results/DBN/Dim10/Dim10.xlsx
+++ b/results/DBN/Dim10/Dim10.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6:G7"/>
@@ -3587,6 +3587,702 @@
         <v>90</v>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>10</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D110" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E110" t="n">
+        <v>485.389730671534</v>
+      </c>
+      <c r="F110" t="n">
+        <v>4.622759339728895</v>
+      </c>
+      <c r="G110" t="n">
+        <v>1.58613062912976</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>10</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>457.3696527705521</v>
+      </c>
+      <c r="F111" t="n">
+        <v>4.234904192319927</v>
+      </c>
+      <c r="G111" t="n">
+        <v>2.339443072459451</v>
+      </c>
+      <c r="H111" t="n">
+        <v>9</v>
+      </c>
+      <c r="I111" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>10</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E112" t="n">
+        <v>456.2853832857861</v>
+      </c>
+      <c r="F112" t="n">
+        <v>4.517677062235506</v>
+      </c>
+      <c r="G112" t="n">
+        <v>1.322501343264093</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0</v>
+      </c>
+      <c r="I112" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>10</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D113" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E113" t="n">
+        <v>126.4616004450432</v>
+      </c>
+      <c r="F113" t="n">
+        <v>1.227782528592652</v>
+      </c>
+      <c r="G113" t="n">
+        <v>1.512833952334825</v>
+      </c>
+      <c r="H113" t="n">
+        <v>37</v>
+      </c>
+      <c r="I113" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>10</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>301.4240134172564</v>
+      </c>
+      <c r="F114" t="n">
+        <v>2.667469145285455</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1.811860493372949</v>
+      </c>
+      <c r="H114" t="n">
+        <v>11</v>
+      </c>
+      <c r="I114" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>10</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E115" t="n">
+        <v>160</v>
+      </c>
+      <c r="F115" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G115" t="n">
+        <v>1.113552872566004</v>
+      </c>
+      <c r="H115" t="n">
+        <v>17</v>
+      </c>
+      <c r="I115" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>10</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D116" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E116" t="n">
+        <v>235.3293326975517</v>
+      </c>
+      <c r="F116" t="n">
+        <v>2.353293326975517</v>
+      </c>
+      <c r="G116" t="n">
+        <v>2.615723708118364</v>
+      </c>
+      <c r="H116" t="n">
+        <v>33</v>
+      </c>
+      <c r="I116" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>10</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>413.2352620545445</v>
+      </c>
+      <c r="F117" t="n">
+        <v>3.862011794902285</v>
+      </c>
+      <c r="G117" t="n">
+        <v>1.943309980698489</v>
+      </c>
+      <c r="H117" t="n">
+        <v>2</v>
+      </c>
+      <c r="I117" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>10</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E118" t="n">
+        <v>441.0037963869226</v>
+      </c>
+      <c r="F118" t="n">
+        <v>4.410037963869226</v>
+      </c>
+      <c r="G118" t="n">
+        <v>1.353353300964745</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>10</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D119" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E119" t="n">
+        <v>446.4981963964198</v>
+      </c>
+      <c r="F119" t="n">
+        <v>4.212247135815281</v>
+      </c>
+      <c r="G119" t="n">
+        <v>1.150222501373096</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>10</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>275.3303953583768</v>
+      </c>
+      <c r="F120" t="n">
+        <v>2.525966929893365</v>
+      </c>
+      <c r="G120" t="n">
+        <v>1.60138852172902</v>
+      </c>
+      <c r="H120" t="n">
+        <v>21</v>
+      </c>
+      <c r="I120" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>10</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E121" t="n">
+        <v>508.2902449861257</v>
+      </c>
+      <c r="F121" t="n">
+        <v>4.88740620178967</v>
+      </c>
+      <c r="G121" t="n">
+        <v>1.134168215823737</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>10</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D122" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E122" t="n">
+        <v>225.0418148726914</v>
+      </c>
+      <c r="F122" t="n">
+        <v>1.771982794273161</v>
+      </c>
+      <c r="G122" t="n">
+        <v>1.540093503791875</v>
+      </c>
+      <c r="H122" t="n">
+        <v>27</v>
+      </c>
+      <c r="I122" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>10</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>366.8478360995956</v>
+      </c>
+      <c r="F123" t="n">
+        <v>2.565369483213955</v>
+      </c>
+      <c r="G123" t="n">
+        <v>1.378911489948525</v>
+      </c>
+      <c r="H123" t="n">
+        <v>12</v>
+      </c>
+      <c r="I123" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>10</v>
+      </c>
+      <c r="B124" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E124" t="n">
+        <v>570.6887643979227</v>
+      </c>
+      <c r="F124" t="n">
+        <v>4.076348317128019</v>
+      </c>
+      <c r="G124" t="n">
+        <v>1.772153281911704</v>
+      </c>
+      <c r="H124" t="n">
+        <v>3</v>
+      </c>
+      <c r="I124" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>10</v>
+      </c>
+      <c r="B125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E125" t="n">
+        <v>408.5878704683959</v>
+      </c>
+      <c r="F125" t="n">
+        <v>4.005763435964666</v>
+      </c>
+      <c r="G125" t="n">
+        <v>1.143153739249074</v>
+      </c>
+      <c r="H125" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>10</v>
+      </c>
+      <c r="B126" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>418.5036749515784</v>
+      </c>
+      <c r="F126" t="n">
+        <v>3.770303377942148</v>
+      </c>
+      <c r="G126" t="n">
+        <v>1.557065213122966</v>
+      </c>
+      <c r="H126" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>10</v>
+      </c>
+      <c r="B127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E127" t="n">
+        <v>514.3652568658816</v>
+      </c>
+      <c r="F127" t="n">
+        <v>4.898716732056015</v>
+      </c>
+      <c r="G127" t="n">
+        <v>1.126605985134598</v>
+      </c>
+      <c r="H127" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>10</v>
+      </c>
+      <c r="B128" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E128" t="n">
+        <v>762.8841343678141</v>
+      </c>
+      <c r="F128" t="n">
+        <v>7.628841343678141</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0.8722268930657734</v>
+      </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>10</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C129" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
+        <v>732.5759519670314</v>
+      </c>
+      <c r="F129" t="n">
+        <v>7.182117176147367</v>
+      </c>
+      <c r="G129" t="n">
+        <v>1.443557942985183</v>
+      </c>
+      <c r="H129" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>10</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C130" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E130" t="n">
+        <v>342.5029183196256</v>
+      </c>
+      <c r="F130" t="n">
+        <v>3.425029183196256</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0.9215069691836295</v>
+      </c>
+      <c r="H130" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>10</v>
+      </c>
+      <c r="B131" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D131" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="E131" t="n">
+        <v>452.2221081874419</v>
+      </c>
+      <c r="F131" t="n">
+        <v>3.932366158151669</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0.8059403678215855</v>
+      </c>
+      <c r="H131" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>10</v>
+      </c>
+      <c r="B132" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>476.4012685208576</v>
+      </c>
+      <c r="F132" t="n">
+        <v>4.253582754650514</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0.8535000414577344</v>
+      </c>
+      <c r="H132" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>10</v>
+      </c>
+      <c r="B133" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D133" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E133" t="n">
+        <v>432.3106080000993</v>
+      </c>
+      <c r="F133" t="n">
+        <v>3.632862252101675</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0.7640840675584952</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="n">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>

</xml_diff>